<commit_message>
Imported immaterial entity [BFO:0000141]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -548,7 +548,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,7 +575,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -636,7 +634,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -664,7 +661,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -692,7 +688,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -720,7 +715,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -748,7 +742,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -776,7 +769,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -804,7 +796,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -832,7 +823,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -860,7 +850,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -888,7 +877,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -916,7 +904,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -944,7 +931,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -972,7 +958,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -992,7 +977,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>material entity [BFO:0000040]; temporal region [BFO:0000008]; site [BFO:0000029]; generically dependent continuant [BFO:0000031]; process [BFO:0000015]; fiat object part [BFO:0000024]</t>
+          <t>temporal region [BFO:0000008]; generically dependent continuant [BFO:0000031]; process [BFO:0000015]; material entity [BFO:0000040]; immaterial entity [BFO:0000141]; site [BFO:0000029]; fiat object part [BFO:0000024]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1000,7 +985,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1028,7 +1012,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1056,7 +1039,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Imported specifically dependent continuant [BFO:0000020]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -548,7 +548,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,7 +575,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -636,7 +634,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -664,7 +661,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -692,7 +688,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -720,7 +715,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -748,7 +742,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -776,7 +769,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -804,7 +796,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -832,7 +823,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -860,7 +850,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -888,7 +877,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -916,7 +904,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -944,7 +931,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -972,7 +958,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -992,7 +977,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>temporal region [BFO:0000008]; generically dependent continuant [BFO:0000031]; process [BFO:0000015]; material entity [BFO:0000040]; immaterial entity [BFO:0000141]; site [BFO:0000029]; fiat object part [BFO:0000024]</t>
+          <t>generically dependent continuant [BFO:0000031]; temporal region [BFO:0000008]; process [BFO:0000015]; material entity [BFO:0000040]; immaterial entity [BFO:0000141]; site [BFO:0000029]; fiat object part [BFO:0000024]; specifically dependent continuant [BFO:0000020]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1000,7 +985,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1028,7 +1012,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1056,7 +1039,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1064,7 +1046,6 @@
           <t>PATO</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>entity [BFO:0000001]</t>
@@ -1080,7 +1061,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Imported extended organism [OGMS:0000087]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -548,7 +548,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,7 +575,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -636,7 +634,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -664,7 +661,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -692,7 +688,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -720,7 +715,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -748,7 +742,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -768,7 +761,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>health care process [OGMS:0000096]; bodily process [OGMS:0000060]; psychotic disorder symptom [OGMS:0000020]; diagnosis [OGMS:0000073]; clinical history [OGMS:0000015]</t>
+          <t>health care process [OGMS:0000096]; bodily process [OGMS:0000060]; extended organism [OGMS:0000087]; psychotic disorder symptom [OGMS:0000020]; diagnosis [OGMS:0000073]; clinical history [OGMS:0000015]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -776,7 +769,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -804,7 +796,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -832,7 +823,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -860,7 +850,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -888,7 +877,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -916,7 +904,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -944,7 +931,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -972,7 +958,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1000,7 +985,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1028,7 +1012,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1056,7 +1039,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1064,7 +1046,6 @@
           <t>PATO</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>entity [BFO:0000001]</t>
@@ -1080,7 +1061,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Imported individual human behaviour pattern [BCIO:036100]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>community healthcare facility [BCIO:026019]; alimentary mode of delivery [BCIO:011037]; ambulance [BCIO:026045]; wearable ingestion mode of delivery [BCIO:011046]; transportation [BCIO:026041]; BCI attribute [BCIO:050315]; inhalation mode of delivery [BCIO:011041]; regular intervention schedule [BCIO:008535]; office facility [BCIO:026037]; country of intervention [BCIO:026001]; transdermal mode of delivery [BCIO:011036]; intervention setting [BCIO:014000]; water [BCIO:026047]; human age [BCIO:015015]; criminal justice facility [BCIO:026038]; irregular intervention schedule [BCIO:008540]; intervention evaluation finding [BCIO:023000]; belief about quality of life [BCIO:050324]; mean human age [BCIO:015177]; psychiatric facility [BCIO:026051]; biological sex [BCIO:015105]; military facility [BCIO:026040]; intervention effect estimate [BCIO:017000]; mobile intervention venue [BCIO:026044]; care home facility [BCIO:026017]; behaviour change intervention source [BCIO:010000]; doctor-led primary care facility [BCIO:026016]; male biological sex [BCIO:015107]; injection mode of delivery [BCIO:011042]; outdoor environment [BCIO:026046]; factory facility [BCIO:026039]; individual human behaviour [BCIO:036000]; evaluation finding [BCIO:035000]; path or pavement [BCIO:026048]; ingestion mode of delivery [BCIO:011035]; medication use status [BCIO:015490]; educational facility [BCIO:026022]; private transportation [BCIO:026043]; female biological sex [BCIO:015106]; study recruitment setting [BCIO:014000]; retail facility [BCIO:026036]; dentist facility [BCIO:026021]; public transportation [BCIO:026042]; community outpatient clinic facility [BCIO:026020]; behaviour change intervention mode of delivery [BCIO:011000]; buccal mode of delivery [BCIO:011040]; community facility [BCIO:026029]; somatic mode of delivery [BCIO:011034]; personal attribute [BCIO:050300]; BCI schedule of delivery [BCIO:008500]; associative learning [BCIO:006119]; experience-related behaviour [BCIO:050443]</t>
+          <t>intervention setting [BCIO:014000]; factory facility [BCIO:026039]; mobile intervention venue [BCIO:026044]; belief about quality of life [BCIO:050324]; associative learning [BCIO:006119]; somatic mode of delivery [BCIO:011034]; transdermal mode of delivery [BCIO:011036]; personal attribute [BCIO:050300]; private transportation [BCIO:026043]; water [BCIO:026047]; irregular intervention schedule [BCIO:008540]; mean human age [BCIO:015177]; BCI attribute [BCIO:050315]; retail facility [BCIO:026036]; behaviour change intervention source [BCIO:010000]; path or pavement [BCIO:026048]; doctor-led primary care facility [BCIO:026016]; care home facility [BCIO:026017]; male biological sex [BCIO:015107]; ingestion mode of delivery [BCIO:011035]; wearable ingestion mode of delivery [BCIO:011046]; study recruitment setting [BCIO:014000]; alimentary mode of delivery [BCIO:011037]; buccal mode of delivery [BCIO:011040]; dentist facility [BCIO:026021]; regular intervention schedule [BCIO:008535]; evaluation finding [BCIO:035000]; educational facility [BCIO:026022]; inhalation mode of delivery [BCIO:011041]; ambulance [BCIO:026045]; individual human behaviour [BCIO:036000]; office facility [BCIO:026037]; medication use status [BCIO:015490]; female biological sex [BCIO:015106]; psychiatric facility [BCIO:026051]; community healthcare facility [BCIO:026019]; intervention effect estimate [BCIO:017000]; criminal justice facility [BCIO:026038]; behaviour change intervention mode of delivery [BCIO:011000]; community outpatient clinic facility [BCIO:026020]; experience-related behaviour [BCIO:050443]; intervention evaluation finding [BCIO:023000]; military facility [BCIO:026040]; public transportation [BCIO:026042]; transportation [BCIO:026041]; human age [BCIO:015015]; BCI schedule of delivery [BCIO:008500]; country of intervention [BCIO:026001]; community facility [BCIO:026029]; injection mode of delivery [BCIO:011042]; outdoor environment [BCIO:026046]; individual human behaviour pattern [BCIO:036100]; biological sex [BCIO:015105]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -548,7 +548,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,7 +575,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -636,7 +634,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -664,7 +661,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -692,7 +688,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -720,7 +715,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -748,7 +742,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -776,7 +769,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -804,7 +796,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -832,7 +823,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -860,7 +850,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -888,7 +877,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -916,7 +904,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -944,7 +931,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -972,7 +958,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1000,7 +985,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1028,7 +1012,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1056,7 +1039,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1084,7 +1066,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>